<commit_message>
Adjusted burndown to account for EmployeeManagement class
</commit_message>
<xml_diff>
--- a/ThomasonCSE248FinalProject/Burndown.xlsx
+++ b/ThomasonCSE248FinalProject/Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hywok\GitFolders\CSE248\ThomasonCSE248FinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\CSE248\CSE248\ThomasonCSE248FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9129C0E1-82D8-4E84-8BF5-187A50AFF702}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4B0EFD-E88F-4842-A29C-847720FB11F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15435" xr2:uid="{6958849C-9034-451C-846B-3BF41C57CBCD}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16749" xr2:uid="{6958849C-9034-451C-846B-3BF41C57CBCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Task</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Time Values</t>
+  </si>
+  <si>
+    <t>Employee Management Class</t>
+  </si>
+  <si>
+    <t>The employee "Bag", data structure TBD</t>
   </si>
 </sst>
 </file>
@@ -257,6 +263,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Time Commitment(h)</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -269,40 +278,84 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$2:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Vehicle/VehicleType Creation.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Burndown Creation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Employee Class</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Employee Management Class</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Garage/Space Classes</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Ticket/Receipt Classes</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Attendant Class</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Manager Class</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Android Studio Study</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Initial design created</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Backend linked to frontend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$B$26</c:f>
+              <c:f>Sheet1!$B$18:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>44</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.5</c:v>
+                  <c:v>45.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -312,65 +365,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C1F0-48CA-BA42-F24067407E11}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$2:$C$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C1F0-48CA-BA42-F24067407E11}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -393,6 +387,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1137,14 +1132,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>92528</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1472,17 +1467,17 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.84375" customWidth="1"/>
+    <col min="4" max="4" width="51.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1496,7 +1491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>43563</v>
       </c>
@@ -1510,7 +1505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>43565</v>
       </c>
@@ -1524,7 +1519,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>43565</v>
       </c>
@@ -1538,222 +1533,237 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
+        <v>43566</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" s="1">
         <v>43568</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" s="1">
         <v>43570</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>43572</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
-        <v>43574</v>
+        <v>43572</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" s="1">
+        <v>43574</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" s="1">
         <v>43579</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>3</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12" s="1">
         <v>43557</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="D12" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A13" s="1"/>
+      <c r="D13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A14" s="1">
         <v>43601</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B14">
-        <f>SUM(B2:B11)</f>
+      <c r="B15">
+        <f>SUM(B2:B12)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" s="1"/>
+      <c r="B18">
+        <f>VALUE($B$15)-B2</f>
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17">
-        <f>VALUE($B$14)-B2</f>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <f>B17-B3</f>
-        <v>42.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B19">
-        <f t="shared" ref="B19:B26" si="0">B18-B4</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+        <f>B18-B3</f>
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B20">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" ref="B20:B28" si="0">B19-B4</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21" s="1"/>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22" s="1"/>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A23" s="1"/>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A24" s="1"/>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A25" s="1"/>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
       <c r="B26">
         <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27" s="1"/>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28" s="1"/>
+      <c r="B28">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A33" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented receipt, TODO early bird pricing
</commit_message>
<xml_diff>
--- a/ThomasonCSE248FinalProject/Burndown.xlsx
+++ b/ThomasonCSE248FinalProject/Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\CSE248\CSE248\ThomasonCSE248FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4B0EFD-E88F-4842-A29C-847720FB11F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED8E41E-4F99-4305-90A8-5C1C09B2179E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16749" xr2:uid="{6958849C-9034-451C-846B-3BF41C57CBCD}"/>
+    <workbookView xWindow="6429" yWindow="1294" windowWidth="19285" windowHeight="12120" xr2:uid="{6958849C-9034-451C-846B-3BF41C57CBCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1467,7 +1467,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1633,7 +1633,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
-        <v>43557</v>
+        <v>43587</v>
       </c>
       <c r="B12">
         <v>15</v>

</xml_diff>